<commit_message>
plots for presentation are made
</commit_message>
<xml_diff>
--- a/Initial table.xlsx
+++ b/Initial table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rudko\Documents\GitHub\PaleoCalc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Дмитрий\Documents\GitHub\PaleoCalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810E8A51-4C88-47B0-A8BB-458177FCE153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8460C3F0-B6F2-4DC8-B0F6-F8725AB84628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23655" yWindow="3960" windowWidth="12765" windowHeight="15435" firstSheet="2" activeTab="2" xr2:uid="{A9179D02-FDD0-4AE1-BE79-EB2273F263CB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{A9179D02-FDD0-4AE1-BE79-EB2273F263CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial" sheetId="1" r:id="rId1"/>
@@ -532,9 +532,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office 2013–2022">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -572,7 +572,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -678,7 +678,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -820,7 +820,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2789,20 +2789,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25778464-7BC4-4097-81C5-41E70C7FD531}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:S41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>110</v>
       </c>
@@ -2815,13 +2815,44 @@
       <c r="D2">
         <v>7.8</v>
       </c>
-      <c r="E2" s="9"/>
+      <c r="E2" s="9">
+        <v>2</v>
+      </c>
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="11">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>-37.925411489356151</v>
+      </c>
+      <c r="J2">
+        <v>327.16469500201845</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>-37.925411489356151</v>
+      </c>
+      <c r="N2">
+        <v>327.16469500201845</v>
+      </c>
+      <c r="O2" s="9">
+        <v>2</v>
+      </c>
+      <c r="Q2">
+        <v>-37.925411489356151</v>
+      </c>
+      <c r="R2">
+        <v>327.16469500201845</v>
+      </c>
+      <c r="S2" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>111</v>
       </c>
@@ -2834,14 +2865,45 @@
       <c r="D3">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="8">
+        <v>4</v>
+      </c>
       <c r="F3">
-        <f>1+F2</f>
+        <f t="shared" ref="F3:F41" si="0">1+F2</f>
         <v>1</v>
       </c>
-      <c r="G3" s="11"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="11">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>-50.018492095268044</v>
+      </c>
+      <c r="J3">
+        <v>292.11718966129882</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>-50.018492095268044</v>
+      </c>
+      <c r="N3">
+        <v>292.11718966129882</v>
+      </c>
+      <c r="O3" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q3">
+        <v>-50.018492095268044</v>
+      </c>
+      <c r="R3">
+        <v>292.11718966129882</v>
+      </c>
+      <c r="S3" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>112</v>
       </c>
@@ -2854,14 +2916,45 @@
       <c r="D4">
         <v>7</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
       <c r="F4">
-        <f>1+F3</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G4" s="11"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="11">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>-63.354516328290977</v>
+      </c>
+      <c r="J4">
+        <v>301.17246047329724</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>-63.354516328290977</v>
+      </c>
+      <c r="N4">
+        <v>301.17246047329724</v>
+      </c>
+      <c r="O4" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>-63.354516328290977</v>
+      </c>
+      <c r="R4">
+        <v>301.17246047329724</v>
+      </c>
+      <c r="S4" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>113</v>
       </c>
@@ -2874,14 +2967,45 @@
       <c r="D5">
         <v>9.6</v>
       </c>
-      <c r="E5" s="8"/>
+      <c r="E5" s="8">
+        <v>4</v>
+      </c>
       <c r="F5">
-        <f>1+F4</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G5" s="11"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="11">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>-51.03063463353574</v>
+      </c>
+      <c r="J5">
+        <v>297.33534359976517</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>-51.03063463353574</v>
+      </c>
+      <c r="N5">
+        <v>297.33534359976517</v>
+      </c>
+      <c r="O5" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q5">
+        <v>-51.03063463353574</v>
+      </c>
+      <c r="R5">
+        <v>297.33534359976517</v>
+      </c>
+      <c r="S5" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>114</v>
       </c>
@@ -2894,14 +3018,45 @@
       <c r="D6">
         <v>9.3000000000000007</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
       <c r="F6">
-        <f>1+F5</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="11">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>-62.457396853265998</v>
+      </c>
+      <c r="J6">
+        <v>345.38443567333286</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>-62.457396853265998</v>
+      </c>
+      <c r="N6">
+        <v>345.38443567333286</v>
+      </c>
+      <c r="O6" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>-62.457396853265998</v>
+      </c>
+      <c r="R6">
+        <v>345.38443567333286</v>
+      </c>
+      <c r="S6" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>115</v>
       </c>
@@ -2914,14 +3069,45 @@
       <c r="D7">
         <v>5.8</v>
       </c>
-      <c r="E7" s="10"/>
+      <c r="E7" s="10">
+        <v>3</v>
+      </c>
       <c r="F7">
-        <f>1+F6</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="11">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>-54.508130149464762</v>
+      </c>
+      <c r="J7">
+        <v>353.19848103384902</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>-54.508130149464762</v>
+      </c>
+      <c r="N7">
+        <v>353.19848103384902</v>
+      </c>
+      <c r="O7" s="10">
+        <v>3</v>
+      </c>
+      <c r="Q7">
+        <v>-54.508130149464762</v>
+      </c>
+      <c r="R7">
+        <v>353.19848103384902</v>
+      </c>
+      <c r="S7" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -2934,14 +3120,45 @@
       <c r="D8">
         <v>4.5</v>
       </c>
-      <c r="E8" s="10"/>
+      <c r="E8" s="10">
+        <v>3</v>
+      </c>
       <c r="F8">
-        <f>1+F7</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G8" s="11"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="11">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>-41.637018278077356</v>
+      </c>
+      <c r="J8">
+        <v>345.92201507584002</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>-41.637018278077356</v>
+      </c>
+      <c r="N8">
+        <v>345.92201507584002</v>
+      </c>
+      <c r="O8" s="10">
+        <v>3</v>
+      </c>
+      <c r="Q8">
+        <v>-41.637018278077356</v>
+      </c>
+      <c r="R8">
+        <v>345.92201507584002</v>
+      </c>
+      <c r="S8" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -2954,14 +3171,45 @@
       <c r="D9">
         <v>5.5</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="5">
+        <v>1</v>
+      </c>
       <c r="F9">
-        <f>1+F8</f>
-        <v>7</v>
-      </c>
-      <c r="G9" s="11"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G9" s="11">
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <v>-64.433623001908046</v>
+      </c>
+      <c r="J9">
+        <v>328.8839512806008</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>-64.433623001908046</v>
+      </c>
+      <c r="N9">
+        <v>328.8839512806008</v>
+      </c>
+      <c r="O9" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>-64.433623001908046</v>
+      </c>
+      <c r="R9">
+        <v>328.8839512806008</v>
+      </c>
+      <c r="S9" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -2974,14 +3222,45 @@
       <c r="D10">
         <v>5.9</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
       <c r="F10">
-        <f>1+F9</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G10" s="12"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" s="12">
+        <v>6</v>
+      </c>
+      <c r="I10">
+        <v>44.225069392695879</v>
+      </c>
+      <c r="J10">
+        <v>127.69563622805951</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>44.225069392695879</v>
+      </c>
+      <c r="N10">
+        <v>127.69563622805951</v>
+      </c>
+      <c r="O10" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>44.225069392695879</v>
+      </c>
+      <c r="R10">
+        <v>127.69563622805951</v>
+      </c>
+      <c r="S10" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
@@ -2994,14 +3273,45 @@
       <c r="D11">
         <v>5.9</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
       <c r="F11">
-        <f>1+F10</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="12">
+        <v>6</v>
+      </c>
+      <c r="I11">
+        <v>48.88111645701418</v>
+      </c>
+      <c r="J11">
+        <v>120.13774169293937</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>48.88111645701418</v>
+      </c>
+      <c r="N11">
+        <v>120.13774169293937</v>
+      </c>
+      <c r="O11" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>48.88111645701418</v>
+      </c>
+      <c r="R11">
+        <v>120.13774169293937</v>
+      </c>
+      <c r="S11" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
@@ -3014,14 +3324,45 @@
       <c r="D12">
         <v>9.6999999999999993</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
       <c r="F12">
-        <f>1+F11</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G12" s="12"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" s="12">
+        <v>6</v>
+      </c>
+      <c r="I12">
+        <v>43.64487257395178</v>
+      </c>
+      <c r="J12">
+        <v>115.90269506029901</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>43.64487257395178</v>
+      </c>
+      <c r="N12">
+        <v>115.90269506029901</v>
+      </c>
+      <c r="O12" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>43.64487257395178</v>
+      </c>
+      <c r="R12">
+        <v>115.90269506029901</v>
+      </c>
+      <c r="S12" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>116</v>
       </c>
@@ -3034,14 +3375,45 @@
       <c r="D13">
         <v>8.4</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
       <c r="F13">
-        <f>1+F12</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="G13" s="12"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="12">
+        <v>6</v>
+      </c>
+      <c r="I13">
+        <v>56.145848752140388</v>
+      </c>
+      <c r="J13">
+        <v>117.77428517501654</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>56.145848752140388</v>
+      </c>
+      <c r="N13">
+        <v>117.77428517501654</v>
+      </c>
+      <c r="O13" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>56.145848752140388</v>
+      </c>
+      <c r="R13">
+        <v>117.77428517501654</v>
+      </c>
+      <c r="S13" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>117</v>
       </c>
@@ -3054,14 +3426,45 @@
       <c r="D14">
         <v>12.3</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="4">
+        <v>0</v>
+      </c>
       <c r="F14">
-        <f>1+F13</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14" s="12">
+        <v>6</v>
+      </c>
+      <c r="I14">
+        <v>61.621979388800746</v>
+      </c>
+      <c r="J14">
+        <v>126.62793530818774</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>61.621979388800746</v>
+      </c>
+      <c r="N14">
+        <v>126.62793530818774</v>
+      </c>
+      <c r="O14" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>61.621979388800746</v>
+      </c>
+      <c r="R14">
+        <v>126.62793530818774</v>
+      </c>
+      <c r="S14" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>118</v>
       </c>
@@ -3074,14 +3477,45 @@
       <c r="D15">
         <v>7.9</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
       <c r="F15">
-        <f>1+F14</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="G15" s="12"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" s="12">
+        <v>6</v>
+      </c>
+      <c r="I15">
+        <v>57.961265277671075</v>
+      </c>
+      <c r="J15">
+        <v>133.23666584153585</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>57.961265277671075</v>
+      </c>
+      <c r="N15">
+        <v>133.23666584153585</v>
+      </c>
+      <c r="O15" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>57.961265277671075</v>
+      </c>
+      <c r="R15">
+        <v>133.23666584153585</v>
+      </c>
+      <c r="S15" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>119</v>
       </c>
@@ -3094,14 +3528,45 @@
       <c r="D16">
         <v>11.9</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
       <c r="F16">
-        <f>1+F15</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="G16" s="12"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="12">
+        <v>6</v>
+      </c>
+      <c r="I16">
+        <v>59.613926395651625</v>
+      </c>
+      <c r="J16">
+        <v>153.13777236927734</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>59.613926395651625</v>
+      </c>
+      <c r="N16">
+        <v>153.13777236927734</v>
+      </c>
+      <c r="O16" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>59.613926395651625</v>
+      </c>
+      <c r="R16">
+        <v>153.13777236927734</v>
+      </c>
+      <c r="S16" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>44</v>
       </c>
@@ -3114,14 +3579,45 @@
       <c r="D17">
         <v>3.3</v>
       </c>
-      <c r="E17" s="4"/>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
       <c r="F17">
-        <f>1+F16</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="12">
+        <v>6</v>
+      </c>
+      <c r="I17">
+        <v>53.394664590935413</v>
+      </c>
+      <c r="J17">
+        <v>125.96484160699701</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>53.394664590935413</v>
+      </c>
+      <c r="N17">
+        <v>125.96484160699701</v>
+      </c>
+      <c r="O17" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>53.394664590935413</v>
+      </c>
+      <c r="R17">
+        <v>125.96484160699701</v>
+      </c>
+      <c r="S17" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>50</v>
       </c>
@@ -3134,14 +3630,45 @@
       <c r="D18">
         <v>14.1</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="E18" s="4">
+        <v>0</v>
+      </c>
       <c r="F18">
-        <f>1+F17</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="13">
+        <v>7</v>
+      </c>
+      <c r="I18">
+        <v>61.763762829987172</v>
+      </c>
+      <c r="J18">
+        <v>153.1845205130322</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>61.763762829987172</v>
+      </c>
+      <c r="N18">
+        <v>153.1845205130322</v>
+      </c>
+      <c r="O18" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>61.763762829987172</v>
+      </c>
+      <c r="R18">
+        <v>153.1845205130322</v>
+      </c>
+      <c r="S18" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
@@ -3154,14 +3681,45 @@
       <c r="D19">
         <v>8.6</v>
       </c>
-      <c r="E19" s="4"/>
+      <c r="E19" s="4">
+        <v>0</v>
+      </c>
       <c r="F19">
-        <f>1+F18</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="G19" s="13"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="13">
+        <v>7</v>
+      </c>
+      <c r="I19">
+        <v>68.71976926357685</v>
+      </c>
+      <c r="J19">
+        <v>125.67083251805261</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>68.71976926357685</v>
+      </c>
+      <c r="N19">
+        <v>125.67083251805261</v>
+      </c>
+      <c r="O19" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>68.71976926357685</v>
+      </c>
+      <c r="R19">
+        <v>125.67083251805261</v>
+      </c>
+      <c r="S19" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>54</v>
       </c>
@@ -3174,14 +3732,45 @@
       <c r="D20">
         <v>3.6</v>
       </c>
-      <c r="E20" s="4"/>
+      <c r="E20" s="4">
+        <v>0</v>
+      </c>
       <c r="F20">
-        <f>1+F19</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="G20" s="13"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="13">
+        <v>7</v>
+      </c>
+      <c r="I20">
+        <v>61.880099106807535</v>
+      </c>
+      <c r="J20">
+        <v>138.81513908883085</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>61.880099106807535</v>
+      </c>
+      <c r="N20">
+        <v>138.81513908883085</v>
+      </c>
+      <c r="O20" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>61.880099106807535</v>
+      </c>
+      <c r="R20">
+        <v>138.81513908883085</v>
+      </c>
+      <c r="S20" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>59</v>
       </c>
@@ -3194,14 +3783,45 @@
       <c r="D21">
         <v>7.6</v>
       </c>
-      <c r="E21" s="10"/>
+      <c r="E21" s="10">
+        <v>3</v>
+      </c>
       <c r="F21">
-        <f>1+F20</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="G21" s="13"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="13">
+        <v>7</v>
+      </c>
+      <c r="I21">
+        <v>-49.043299948858987</v>
+      </c>
+      <c r="J21">
+        <v>350.13417741133674</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>-49.043299948858987</v>
+      </c>
+      <c r="N21">
+        <v>350.13417741133674</v>
+      </c>
+      <c r="O21" s="10">
+        <v>3</v>
+      </c>
+      <c r="Q21">
+        <v>-49.043299948858987</v>
+      </c>
+      <c r="R21">
+        <v>350.13417741133674</v>
+      </c>
+      <c r="S21" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>60</v>
       </c>
@@ -3214,14 +3834,45 @@
       <c r="D22">
         <v>9</v>
       </c>
-      <c r="E22" s="10"/>
+      <c r="E22" s="10">
+        <v>3</v>
+      </c>
       <c r="F22">
-        <f>1+F21</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G22" s="13"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="13">
+        <v>7</v>
+      </c>
+      <c r="I22">
+        <v>-32.639143116367705</v>
+      </c>
+      <c r="J22">
+        <v>343.68240176956448</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>-32.639143116367705</v>
+      </c>
+      <c r="N22">
+        <v>343.68240176956448</v>
+      </c>
+      <c r="O22" s="10">
+        <v>3</v>
+      </c>
+      <c r="Q22">
+        <v>-32.639143116367705</v>
+      </c>
+      <c r="R22">
+        <v>343.68240176956448</v>
+      </c>
+      <c r="S22" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>62</v>
       </c>
@@ -3234,14 +3885,45 @@
       <c r="D23">
         <v>9.1</v>
       </c>
-      <c r="E23" s="9"/>
+      <c r="E23" s="9">
+        <v>2</v>
+      </c>
       <c r="F23">
-        <f>1+F22</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="G23" s="13"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="13">
+        <v>7</v>
+      </c>
+      <c r="I23">
+        <v>-47.244701941718738</v>
+      </c>
+      <c r="J23">
+        <v>332.00481016678765</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>-47.244701941718738</v>
+      </c>
+      <c r="N23">
+        <v>332.00481016678765</v>
+      </c>
+      <c r="O23" s="9">
+        <v>2</v>
+      </c>
+      <c r="Q23">
+        <v>-47.244701941718738</v>
+      </c>
+      <c r="R23">
+        <v>332.00481016678765</v>
+      </c>
+      <c r="S23" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>121</v>
       </c>
@@ -3254,14 +3936,45 @@
       <c r="D24">
         <v>6</v>
       </c>
-      <c r="E24" s="9"/>
+      <c r="E24" s="9">
+        <v>2</v>
+      </c>
       <c r="F24">
-        <f>1+F23</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="G24" s="13"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="13">
+        <v>7</v>
+      </c>
+      <c r="I24">
+        <v>-44.495801705094905</v>
+      </c>
+      <c r="J24">
+        <v>320.67615358580292</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>-44.495801705094905</v>
+      </c>
+      <c r="N24">
+        <v>320.67615358580292</v>
+      </c>
+      <c r="O24" s="9">
+        <v>2</v>
+      </c>
+      <c r="Q24">
+        <v>-44.495801705094905</v>
+      </c>
+      <c r="R24">
+        <v>320.67615358580292</v>
+      </c>
+      <c r="S24" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>65</v>
       </c>
@@ -3274,14 +3987,45 @@
       <c r="D25">
         <v>10.4</v>
       </c>
-      <c r="E25" s="9"/>
+      <c r="E25" s="9">
+        <v>2</v>
+      </c>
       <c r="F25">
-        <f>1+F24</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="G25" s="13"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="13">
+        <v>7</v>
+      </c>
+      <c r="I25">
+        <v>-39.724834852503371</v>
+      </c>
+      <c r="J25">
+        <v>316.47069863943852</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>-39.724834852503371</v>
+      </c>
+      <c r="N25">
+        <v>316.47069863943852</v>
+      </c>
+      <c r="O25" s="9">
+        <v>2</v>
+      </c>
+      <c r="Q25">
+        <v>-39.724834852503371</v>
+      </c>
+      <c r="R25">
+        <v>316.47069863943852</v>
+      </c>
+      <c r="S25" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>66</v>
       </c>
@@ -3294,14 +4038,45 @@
       <c r="D26">
         <v>6</v>
       </c>
-      <c r="E26" s="9"/>
+      <c r="E26" s="9">
+        <v>2</v>
+      </c>
       <c r="F26">
-        <f>1+F25</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="G26" s="13"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G26" s="13">
+        <v>7</v>
+      </c>
+      <c r="I26">
+        <v>-77.626557162397077</v>
+      </c>
+      <c r="J26">
+        <v>341.73145435384208</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>-77.626557162397077</v>
+      </c>
+      <c r="N26">
+        <v>341.73145435384208</v>
+      </c>
+      <c r="O26" s="9">
+        <v>2</v>
+      </c>
+      <c r="Q26">
+        <v>-77.626557162397077</v>
+      </c>
+      <c r="R26">
+        <v>341.73145435384208</v>
+      </c>
+      <c r="S26" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>122</v>
       </c>
@@ -3314,14 +4089,45 @@
       <c r="D27">
         <v>10.5</v>
       </c>
-      <c r="E27" s="5"/>
+      <c r="E27" s="5">
+        <v>1</v>
+      </c>
       <c r="F27">
-        <f>1+F26</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="G27" s="13"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="13">
+        <v>7</v>
+      </c>
+      <c r="I27">
+        <v>-71.056534293717277</v>
+      </c>
+      <c r="J27">
+        <v>328.37673685640493</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>-71.056534293717277</v>
+      </c>
+      <c r="N27">
+        <v>328.37673685640493</v>
+      </c>
+      <c r="O27" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <v>-71.056534293717277</v>
+      </c>
+      <c r="R27">
+        <v>328.37673685640493</v>
+      </c>
+      <c r="S27" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>69</v>
       </c>
@@ -3334,14 +4140,45 @@
       <c r="D28">
         <v>8</v>
       </c>
-      <c r="E28" s="9"/>
+      <c r="E28" s="9">
+        <v>2</v>
+      </c>
       <c r="F28">
-        <f>1+F27</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="G28" s="13"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G28" s="13">
+        <v>7</v>
+      </c>
+      <c r="I28">
+        <v>-49.808156241005008</v>
+      </c>
+      <c r="J28">
+        <v>336.45007295084685</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>-49.808156241005008</v>
+      </c>
+      <c r="N28">
+        <v>336.45007295084685</v>
+      </c>
+      <c r="O28" s="9">
+        <v>2</v>
+      </c>
+      <c r="Q28">
+        <v>-49.808156241005008</v>
+      </c>
+      <c r="R28">
+        <v>336.45007295084685</v>
+      </c>
+      <c r="S28" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>71</v>
       </c>
@@ -3354,14 +4191,45 @@
       <c r="D29">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E29" s="8"/>
+      <c r="E29" s="8">
+        <v>4</v>
+      </c>
       <c r="F29">
-        <f>1+F28</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="G29" s="13"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G29" s="13">
+        <v>7</v>
+      </c>
+      <c r="I29">
+        <v>-51.065744717094091</v>
+      </c>
+      <c r="J29">
+        <v>305.27655504587648</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>-51.065744717094091</v>
+      </c>
+      <c r="N29">
+        <v>305.27655504587648</v>
+      </c>
+      <c r="O29" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q29">
+        <v>-51.065744717094091</v>
+      </c>
+      <c r="R29">
+        <v>305.27655504587648</v>
+      </c>
+      <c r="S29" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>72</v>
       </c>
@@ -3374,14 +4242,45 @@
       <c r="D30">
         <v>7.5</v>
       </c>
-      <c r="E30" s="5"/>
+      <c r="E30" s="5">
+        <v>1</v>
+      </c>
       <c r="F30">
-        <f>1+F29</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="G30" s="13"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G30" s="13">
+        <v>7</v>
+      </c>
+      <c r="I30">
+        <v>-62.833710978294256</v>
+      </c>
+      <c r="J30">
+        <v>332.35677431394953</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>-62.833710978294256</v>
+      </c>
+      <c r="N30">
+        <v>332.35677431394953</v>
+      </c>
+      <c r="O30" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q30">
+        <v>-62.833710978294256</v>
+      </c>
+      <c r="R30">
+        <v>332.35677431394953</v>
+      </c>
+      <c r="S30" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>74</v>
       </c>
@@ -3394,14 +4293,45 @@
       <c r="D31">
         <v>8.1999999999999993</v>
       </c>
-      <c r="E31" s="10"/>
+      <c r="E31" s="10">
+        <v>3</v>
+      </c>
       <c r="F31">
-        <f>1+F30</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="G31" s="13"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G31" s="13">
+        <v>7</v>
+      </c>
+      <c r="I31">
+        <v>-44.060143916807128</v>
+      </c>
+      <c r="J31">
+        <v>0.23310846630991477</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>-44.060143916807128</v>
+      </c>
+      <c r="N31">
+        <v>0.23310846630991477</v>
+      </c>
+      <c r="O31" s="10">
+        <v>3</v>
+      </c>
+      <c r="Q31">
+        <v>-44.060143916807128</v>
+      </c>
+      <c r="R31">
+        <v>0.23310846630991477</v>
+      </c>
+      <c r="S31" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>77</v>
       </c>
@@ -3414,14 +4344,45 @@
       <c r="D32">
         <v>7.2</v>
       </c>
-      <c r="E32" s="4"/>
+      <c r="E32" s="4">
+        <v>0</v>
+      </c>
       <c r="F32">
-        <f>1+F31</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="G32" s="13"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G32" s="13">
+        <v>7</v>
+      </c>
+      <c r="I32">
+        <v>55.076595413432102</v>
+      </c>
+      <c r="J32">
+        <v>101.4122131237026</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>55.076595413432102</v>
+      </c>
+      <c r="N32">
+        <v>101.4122131237026</v>
+      </c>
+      <c r="O32" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>55.076595413432102</v>
+      </c>
+      <c r="R32">
+        <v>101.4122131237026</v>
+      </c>
+      <c r="S32" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>78</v>
       </c>
@@ -3434,14 +4395,45 @@
       <c r="D33">
         <v>4.7</v>
       </c>
-      <c r="E33" s="4"/>
+      <c r="E33" s="4">
+        <v>0</v>
+      </c>
       <c r="F33">
-        <f>1+F32</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="G33" s="13"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G33" s="13">
+        <v>7</v>
+      </c>
+      <c r="I33">
+        <v>52.46597646230758</v>
+      </c>
+      <c r="J33">
+        <v>119.9713378441469</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>52.46597646230758</v>
+      </c>
+      <c r="N33">
+        <v>119.9713378441469</v>
+      </c>
+      <c r="O33" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <v>52.46597646230758</v>
+      </c>
+      <c r="R33">
+        <v>119.9713378441469</v>
+      </c>
+      <c r="S33" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>79</v>
       </c>
@@ -3454,14 +4446,45 @@
       <c r="D34">
         <v>9.6999999999999993</v>
       </c>
-      <c r="E34" s="4"/>
+      <c r="E34" s="4">
+        <v>0</v>
+      </c>
       <c r="F34">
-        <f>1+F33</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="G34" s="13"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G34" s="13">
+        <v>7</v>
+      </c>
+      <c r="I34">
+        <v>46.883910019017087</v>
+      </c>
+      <c r="J34">
+        <v>139.31174435364977</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>46.883910019017087</v>
+      </c>
+      <c r="N34">
+        <v>139.31174435364977</v>
+      </c>
+      <c r="O34" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <v>46.883910019017087</v>
+      </c>
+      <c r="R34">
+        <v>139.31174435364977</v>
+      </c>
+      <c r="S34" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>80</v>
       </c>
@@ -3474,14 +4497,45 @@
       <c r="D35">
         <v>7.7</v>
       </c>
-      <c r="E35" s="4"/>
+      <c r="E35" s="4">
+        <v>0</v>
+      </c>
       <c r="F35">
-        <f>1+F34</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="G35" s="13"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G35" s="13">
+        <v>7</v>
+      </c>
+      <c r="I35">
+        <v>46.733315373505363</v>
+      </c>
+      <c r="J35">
+        <v>119.53036363979632</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>46.733315373505363</v>
+      </c>
+      <c r="N35">
+        <v>119.53036363979632</v>
+      </c>
+      <c r="O35" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>46.733315373505363</v>
+      </c>
+      <c r="R35">
+        <v>119.53036363979632</v>
+      </c>
+      <c r="S35" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>81</v>
       </c>
@@ -3494,14 +4548,45 @@
       <c r="D36">
         <v>13.6</v>
       </c>
-      <c r="E36" s="4"/>
+      <c r="E36" s="4">
+        <v>0</v>
+      </c>
       <c r="F36">
-        <f>1+F35</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="G36" s="13"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G36" s="13">
+        <v>7</v>
+      </c>
+      <c r="I36">
+        <v>64.607379122519191</v>
+      </c>
+      <c r="J36">
+        <v>138.42372628168536</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>64.607379122519191</v>
+      </c>
+      <c r="N36">
+        <v>138.42372628168536</v>
+      </c>
+      <c r="O36" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <v>64.607379122519191</v>
+      </c>
+      <c r="R36">
+        <v>138.42372628168536</v>
+      </c>
+      <c r="S36" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>83</v>
       </c>
@@ -3514,14 +4599,45 @@
       <c r="D37">
         <v>11.2</v>
       </c>
-      <c r="E37" s="5"/>
+      <c r="E37" s="5">
+        <v>1</v>
+      </c>
       <c r="F37">
-        <f>1+F36</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="G37" s="13"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G37" s="13">
+        <v>7</v>
+      </c>
+      <c r="I37">
+        <v>-55.975077011423906</v>
+      </c>
+      <c r="J37">
+        <v>344.53513723408918</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>-55.975077011423906</v>
+      </c>
+      <c r="N37">
+        <v>344.53513723408918</v>
+      </c>
+      <c r="O37" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q37">
+        <v>-55.975077011423906</v>
+      </c>
+      <c r="R37">
+        <v>344.53513723408918</v>
+      </c>
+      <c r="S37" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>85</v>
       </c>
@@ -3534,14 +4650,45 @@
       <c r="D38">
         <v>9.6</v>
       </c>
-      <c r="E38" s="4"/>
+      <c r="E38" s="4">
+        <v>0</v>
+      </c>
       <c r="F38">
-        <f>1+F37</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="G38" s="13"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G38" s="13">
+        <v>7</v>
+      </c>
+      <c r="I38">
+        <v>54.22513226980098</v>
+      </c>
+      <c r="J38">
+        <v>102.10546108645241</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <v>54.22513226980098</v>
+      </c>
+      <c r="N38">
+        <v>102.10546108645241</v>
+      </c>
+      <c r="O38" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q38">
+        <v>54.22513226980098</v>
+      </c>
+      <c r="R38">
+        <v>102.10546108645241</v>
+      </c>
+      <c r="S38" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>86</v>
       </c>
@@ -3554,14 +4701,45 @@
       <c r="D39">
         <v>6.1</v>
       </c>
-      <c r="E39" s="4"/>
+      <c r="E39" s="4">
+        <v>0</v>
+      </c>
       <c r="F39">
-        <f>1+F38</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="G39" s="13"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G39" s="13">
+        <v>7</v>
+      </c>
+      <c r="I39">
+        <v>46.274060146584887</v>
+      </c>
+      <c r="J39">
+        <v>102.74642430827177</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>46.274060146584887</v>
+      </c>
+      <c r="N39">
+        <v>102.74642430827177</v>
+      </c>
+      <c r="O39" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q39">
+        <v>46.274060146584887</v>
+      </c>
+      <c r="R39">
+        <v>102.74642430827177</v>
+      </c>
+      <c r="S39" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>88</v>
       </c>
@@ -3574,14 +4752,45 @@
       <c r="D40">
         <v>10.199999999999999</v>
       </c>
-      <c r="E40" s="5"/>
+      <c r="E40" s="5">
+        <v>1</v>
+      </c>
       <c r="F40">
-        <f>1+F39</f>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="G40" s="13"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G40" s="13">
+        <v>7</v>
+      </c>
+      <c r="I40">
+        <v>-62.611046384420206</v>
+      </c>
+      <c r="J40">
+        <v>314.77581486422946</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>-62.611046384420206</v>
+      </c>
+      <c r="N40">
+        <v>314.77581486422946</v>
+      </c>
+      <c r="O40" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q40">
+        <v>-62.611046384420206</v>
+      </c>
+      <c r="R40">
+        <v>314.77581486422946</v>
+      </c>
+      <c r="S40" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>90</v>
       </c>
@@ -3594,12 +4803,43 @@
       <c r="D41">
         <v>9.5</v>
       </c>
-      <c r="E41" s="4"/>
+      <c r="E41" s="4">
+        <v>0</v>
+      </c>
       <c r="F41">
-        <f>1+F40</f>
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="G41" s="13"/>
+      <c r="G41" s="13">
+        <v>7</v>
+      </c>
+      <c r="I41">
+        <v>63.762712081162846</v>
+      </c>
+      <c r="J41">
+        <v>110.43425915639428</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>63.762712081162846</v>
+      </c>
+      <c r="N41">
+        <v>110.43425915639428</v>
+      </c>
+      <c r="O41" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q41">
+        <v>63.762712081162846</v>
+      </c>
+      <c r="R41">
+        <v>110.43425915639428</v>
+      </c>
+      <c r="S41" s="13">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3608,20 +4848,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14CE2E54-C220-49CE-9A06-4CC0FE82E70A}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C41"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G41" sqref="G2:G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>110</v>
       </c>
@@ -3640,9 +4880,38 @@
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="11">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>37.925411490000002</v>
+      </c>
+      <c r="J2">
+        <v>147.16469499999999</v>
+      </c>
+      <c r="K2" s="6">
+        <v>2</v>
+      </c>
+      <c r="M2">
+        <v>37.925411490000002</v>
+      </c>
+      <c r="N2">
+        <v>147.16469499999999</v>
+      </c>
+      <c r="O2" s="11">
+        <v>5</v>
+      </c>
+      <c r="Q2">
+        <v>37.925411490000002</v>
+      </c>
+      <c r="R2">
+        <v>147.16469499999999</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>111</v>
       </c>
@@ -3662,9 +4931,38 @@
         <f>1+F2</f>
         <v>1</v>
       </c>
-      <c r="G3" s="11"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="11">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>50.018492100000003</v>
+      </c>
+      <c r="J3">
+        <v>112.1171897</v>
+      </c>
+      <c r="K3" s="7">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>50.018492100000003</v>
+      </c>
+      <c r="N3">
+        <v>112.1171897</v>
+      </c>
+      <c r="O3" s="11">
+        <v>5</v>
+      </c>
+      <c r="Q3">
+        <v>50.018492100000003</v>
+      </c>
+      <c r="R3">
+        <v>112.1171897</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>112</v>
       </c>
@@ -3684,9 +4982,38 @@
         <f t="shared" ref="F4:F41" si="0">1+F3</f>
         <v>2</v>
       </c>
-      <c r="G4" s="11"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="11">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>63.354516330000003</v>
+      </c>
+      <c r="J4">
+        <v>121.1724605</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>63.354516330000003</v>
+      </c>
+      <c r="N4">
+        <v>121.1724605</v>
+      </c>
+      <c r="O4" s="11">
+        <v>5</v>
+      </c>
+      <c r="Q4">
+        <v>63.354516330000003</v>
+      </c>
+      <c r="R4">
+        <v>121.1724605</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>113</v>
       </c>
@@ -3706,9 +5033,38 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G5" s="11"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="11">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>51.030634630000002</v>
+      </c>
+      <c r="J5">
+        <v>117.3353436</v>
+      </c>
+      <c r="K5" s="7">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>51.030634630000002</v>
+      </c>
+      <c r="N5">
+        <v>117.3353436</v>
+      </c>
+      <c r="O5" s="11">
+        <v>5</v>
+      </c>
+      <c r="Q5">
+        <v>51.030634630000002</v>
+      </c>
+      <c r="R5">
+        <v>117.3353436</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>114</v>
       </c>
@@ -3728,9 +5084,38 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="11">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>62.457396850000002</v>
+      </c>
+      <c r="J6">
+        <v>165.38443570000001</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>62.457396850000002</v>
+      </c>
+      <c r="N6">
+        <v>165.38443570000001</v>
+      </c>
+      <c r="O6" s="11">
+        <v>5</v>
+      </c>
+      <c r="Q6">
+        <v>62.457396850000002</v>
+      </c>
+      <c r="R6">
+        <v>165.38443570000001</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>115</v>
       </c>
@@ -3750,9 +5135,38 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="11">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>54.50813015</v>
+      </c>
+      <c r="J7">
+        <v>173.19848099999999</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>54.50813015</v>
+      </c>
+      <c r="N7">
+        <v>173.19848099999999</v>
+      </c>
+      <c r="O7" s="11">
+        <v>5</v>
+      </c>
+      <c r="Q7">
+        <v>54.50813015</v>
+      </c>
+      <c r="R7">
+        <v>173.19848099999999</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -3772,9 +5186,38 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G8" s="11"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="11">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>41.637018279999999</v>
+      </c>
+      <c r="J8">
+        <v>165.92201510000001</v>
+      </c>
+      <c r="K8" s="3">
+        <v>4</v>
+      </c>
+      <c r="M8">
+        <v>41.637018279999999</v>
+      </c>
+      <c r="N8">
+        <v>165.92201510000001</v>
+      </c>
+      <c r="O8" s="11">
+        <v>5</v>
+      </c>
+      <c r="Q8">
+        <v>41.637018279999999</v>
+      </c>
+      <c r="R8">
+        <v>165.92201510000001</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -3794,9 +5237,38 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="G9" s="11"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="11">
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <v>64.433622999999997</v>
+      </c>
+      <c r="J9">
+        <v>148.88395130000001</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>64.433622999999997</v>
+      </c>
+      <c r="N9">
+        <v>148.88395130000001</v>
+      </c>
+      <c r="O9" s="11">
+        <v>5</v>
+      </c>
+      <c r="Q9">
+        <v>64.433622999999997</v>
+      </c>
+      <c r="R9">
+        <v>148.88395130000001</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -3816,9 +5288,38 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G10" s="12"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" s="12">
+        <v>6</v>
+      </c>
+      <c r="I10">
+        <v>44.225069390000002</v>
+      </c>
+      <c r="J10">
+        <v>127.6956362</v>
+      </c>
+      <c r="K10" s="7">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>44.225069390000002</v>
+      </c>
+      <c r="N10">
+        <v>127.6956362</v>
+      </c>
+      <c r="O10" s="12">
+        <v>6</v>
+      </c>
+      <c r="Q10">
+        <v>44.225069390000002</v>
+      </c>
+      <c r="R10">
+        <v>127.6956362</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
@@ -3838,9 +5339,38 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="12">
+        <v>6</v>
+      </c>
+      <c r="I11">
+        <v>48.881116460000001</v>
+      </c>
+      <c r="J11">
+        <v>120.13774170000001</v>
+      </c>
+      <c r="K11" s="7">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>48.881116460000001</v>
+      </c>
+      <c r="N11">
+        <v>120.13774170000001</v>
+      </c>
+      <c r="O11" s="12">
+        <v>6</v>
+      </c>
+      <c r="Q11">
+        <v>48.881116460000001</v>
+      </c>
+      <c r="R11">
+        <v>120.13774170000001</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
@@ -3860,9 +5390,38 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G12" s="12"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" s="12">
+        <v>6</v>
+      </c>
+      <c r="I12">
+        <v>43.644872569999997</v>
+      </c>
+      <c r="J12">
+        <v>115.9026951</v>
+      </c>
+      <c r="K12" s="7">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>43.644872569999997</v>
+      </c>
+      <c r="N12">
+        <v>115.9026951</v>
+      </c>
+      <c r="O12" s="12">
+        <v>6</v>
+      </c>
+      <c r="Q12">
+        <v>43.644872569999997</v>
+      </c>
+      <c r="R12">
+        <v>115.9026951</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>116</v>
       </c>
@@ -3882,9 +5441,38 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="G13" s="12"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="12">
+        <v>6</v>
+      </c>
+      <c r="I13">
+        <v>56.145848749999999</v>
+      </c>
+      <c r="J13">
+        <v>117.77428519999999</v>
+      </c>
+      <c r="K13" s="7">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>56.145848749999999</v>
+      </c>
+      <c r="N13">
+        <v>117.77428519999999</v>
+      </c>
+      <c r="O13" s="12">
+        <v>6</v>
+      </c>
+      <c r="Q13">
+        <v>56.145848749999999</v>
+      </c>
+      <c r="R13">
+        <v>117.77428519999999</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>117</v>
       </c>
@@ -3904,9 +5492,38 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14" s="12">
+        <v>6</v>
+      </c>
+      <c r="I14">
+        <v>61.62197939</v>
+      </c>
+      <c r="J14">
+        <v>126.6279353</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>61.62197939</v>
+      </c>
+      <c r="N14">
+        <v>126.6279353</v>
+      </c>
+      <c r="O14" s="12">
+        <v>6</v>
+      </c>
+      <c r="Q14">
+        <v>61.62197939</v>
+      </c>
+      <c r="R14">
+        <v>126.6279353</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>118</v>
       </c>
@@ -3926,9 +5543,38 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="G15" s="12"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" s="12">
+        <v>6</v>
+      </c>
+      <c r="I15">
+        <v>57.961265279999999</v>
+      </c>
+      <c r="J15">
+        <v>133.2366658</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>57.961265279999999</v>
+      </c>
+      <c r="N15">
+        <v>133.2366658</v>
+      </c>
+      <c r="O15" s="12">
+        <v>6</v>
+      </c>
+      <c r="Q15">
+        <v>57.961265279999999</v>
+      </c>
+      <c r="R15">
+        <v>133.2366658</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>119</v>
       </c>
@@ -3948,9 +5594,38 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="G16" s="12"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="12">
+        <v>6</v>
+      </c>
+      <c r="I16">
+        <v>59.613926399999997</v>
+      </c>
+      <c r="J16">
+        <v>153.13777239999999</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>59.613926399999997</v>
+      </c>
+      <c r="N16">
+        <v>153.13777239999999</v>
+      </c>
+      <c r="O16" s="12">
+        <v>6</v>
+      </c>
+      <c r="Q16">
+        <v>59.613926399999997</v>
+      </c>
+      <c r="R16">
+        <v>153.13777239999999</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>44</v>
       </c>
@@ -3970,9 +5645,38 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="12">
+        <v>6</v>
+      </c>
+      <c r="I17">
+        <v>53.394664589999998</v>
+      </c>
+      <c r="J17">
+        <v>125.9648416</v>
+      </c>
+      <c r="K17" s="7">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>53.394664589999998</v>
+      </c>
+      <c r="N17">
+        <v>125.9648416</v>
+      </c>
+      <c r="O17" s="12">
+        <v>6</v>
+      </c>
+      <c r="Q17">
+        <v>53.394664589999998</v>
+      </c>
+      <c r="R17">
+        <v>125.9648416</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>50</v>
       </c>
@@ -3992,9 +5696,38 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="13">
+        <v>7</v>
+      </c>
+      <c r="I18">
+        <v>61.763762829999997</v>
+      </c>
+      <c r="J18">
+        <v>153.18452049999999</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>61.763762829999997</v>
+      </c>
+      <c r="N18">
+        <v>153.18452049999999</v>
+      </c>
+      <c r="O18" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q18">
+        <v>61.763762829999997</v>
+      </c>
+      <c r="R18">
+        <v>153.18452049999999</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
@@ -4014,9 +5747,38 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="G19" s="13"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="13">
+        <v>7</v>
+      </c>
+      <c r="I19">
+        <v>68.719769260000007</v>
+      </c>
+      <c r="J19">
+        <v>125.6708325</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>68.719769260000007</v>
+      </c>
+      <c r="N19">
+        <v>125.6708325</v>
+      </c>
+      <c r="O19" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q19">
+        <v>68.719769260000007</v>
+      </c>
+      <c r="R19">
+        <v>125.6708325</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>54</v>
       </c>
@@ -4036,9 +5798,38 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="G20" s="13"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="13">
+        <v>7</v>
+      </c>
+      <c r="I20">
+        <v>61.880099110000003</v>
+      </c>
+      <c r="J20">
+        <v>138.81513910000001</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>61.880099110000003</v>
+      </c>
+      <c r="N20">
+        <v>138.81513910000001</v>
+      </c>
+      <c r="O20" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q20">
+        <v>61.880099110000003</v>
+      </c>
+      <c r="R20">
+        <v>138.81513910000001</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>59</v>
       </c>
@@ -4058,9 +5849,38 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="G21" s="13"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="13">
+        <v>7</v>
+      </c>
+      <c r="I21">
+        <v>49.043299949999998</v>
+      </c>
+      <c r="J21">
+        <v>170.1341774</v>
+      </c>
+      <c r="K21" s="2">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>49.043299949999998</v>
+      </c>
+      <c r="N21">
+        <v>170.1341774</v>
+      </c>
+      <c r="O21" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q21">
+        <v>49.043299949999998</v>
+      </c>
+      <c r="R21">
+        <v>170.1341774</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>60</v>
       </c>
@@ -4080,9 +5900,38 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G22" s="13"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="13">
+        <v>7</v>
+      </c>
+      <c r="I22">
+        <v>32.63914312</v>
+      </c>
+      <c r="J22">
+        <v>163.68240180000001</v>
+      </c>
+      <c r="K22" s="3">
+        <v>4</v>
+      </c>
+      <c r="M22">
+        <v>32.63914312</v>
+      </c>
+      <c r="N22">
+        <v>163.68240180000001</v>
+      </c>
+      <c r="O22" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q22">
+        <v>32.63914312</v>
+      </c>
+      <c r="R22">
+        <v>163.68240180000001</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>62</v>
       </c>
@@ -4102,9 +5951,38 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="G23" s="13"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="13">
+        <v>7</v>
+      </c>
+      <c r="I23">
+        <v>47.244701939999999</v>
+      </c>
+      <c r="J23">
+        <v>152.00481020000001</v>
+      </c>
+      <c r="K23" s="6">
+        <v>2</v>
+      </c>
+      <c r="M23">
+        <v>47.244701939999999</v>
+      </c>
+      <c r="N23">
+        <v>152.00481020000001</v>
+      </c>
+      <c r="O23" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q23">
+        <v>47.244701939999999</v>
+      </c>
+      <c r="R23">
+        <v>152.00481020000001</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>121</v>
       </c>
@@ -4124,9 +6002,38 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="G24" s="13"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="13">
+        <v>7</v>
+      </c>
+      <c r="I24">
+        <v>44.495801710000002</v>
+      </c>
+      <c r="J24">
+        <v>140.67615359999999</v>
+      </c>
+      <c r="K24" s="6">
+        <v>2</v>
+      </c>
+      <c r="M24">
+        <v>44.495801710000002</v>
+      </c>
+      <c r="N24">
+        <v>140.67615359999999</v>
+      </c>
+      <c r="O24" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q24">
+        <v>44.495801710000002</v>
+      </c>
+      <c r="R24">
+        <v>140.67615359999999</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>65</v>
       </c>
@@ -4146,9 +6053,38 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="G25" s="13"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="13">
+        <v>7</v>
+      </c>
+      <c r="I25">
+        <v>39.724834850000001</v>
+      </c>
+      <c r="J25">
+        <v>136.47069859999999</v>
+      </c>
+      <c r="K25" s="6">
+        <v>2</v>
+      </c>
+      <c r="M25">
+        <v>39.724834850000001</v>
+      </c>
+      <c r="N25">
+        <v>136.47069859999999</v>
+      </c>
+      <c r="O25" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q25">
+        <v>39.724834850000001</v>
+      </c>
+      <c r="R25">
+        <v>136.47069859999999</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>66</v>
       </c>
@@ -4168,9 +6104,38 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="G26" s="13"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G26" s="13">
+        <v>7</v>
+      </c>
+      <c r="I26">
+        <v>77.626557160000004</v>
+      </c>
+      <c r="J26">
+        <v>161.73145439999999</v>
+      </c>
+      <c r="K26" s="2">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>77.626557160000004</v>
+      </c>
+      <c r="N26">
+        <v>161.73145439999999</v>
+      </c>
+      <c r="O26" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q26">
+        <v>77.626557160000004</v>
+      </c>
+      <c r="R26">
+        <v>161.73145439999999</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>122</v>
       </c>
@@ -4190,9 +6155,38 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="G27" s="13"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="13">
+        <v>7</v>
+      </c>
+      <c r="I27">
+        <v>71.056534290000002</v>
+      </c>
+      <c r="J27">
+        <v>148.3767369</v>
+      </c>
+      <c r="K27" s="2">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>71.056534290000002</v>
+      </c>
+      <c r="N27">
+        <v>148.3767369</v>
+      </c>
+      <c r="O27" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q27">
+        <v>71.056534290000002</v>
+      </c>
+      <c r="R27">
+        <v>148.3767369</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>69</v>
       </c>
@@ -4212,9 +6206,38 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="G28" s="13"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G28" s="13">
+        <v>7</v>
+      </c>
+      <c r="I28">
+        <v>49.808156240000002</v>
+      </c>
+      <c r="J28">
+        <v>156.450073</v>
+      </c>
+      <c r="K28" s="2">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>49.808156240000002</v>
+      </c>
+      <c r="N28">
+        <v>156.450073</v>
+      </c>
+      <c r="O28" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q28">
+        <v>49.808156240000002</v>
+      </c>
+      <c r="R28">
+        <v>156.450073</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>71</v>
       </c>
@@ -4234,9 +6257,38 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="G29" s="13"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G29" s="13">
+        <v>7</v>
+      </c>
+      <c r="I29">
+        <v>51.065744719999998</v>
+      </c>
+      <c r="J29">
+        <v>125.276555</v>
+      </c>
+      <c r="K29" s="7">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>51.065744719999998</v>
+      </c>
+      <c r="N29">
+        <v>125.276555</v>
+      </c>
+      <c r="O29" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q29">
+        <v>51.065744719999998</v>
+      </c>
+      <c r="R29">
+        <v>125.276555</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>72</v>
       </c>
@@ -4256,9 +6308,38 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="G30" s="13"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G30" s="13">
+        <v>7</v>
+      </c>
+      <c r="I30">
+        <v>62.833710979999999</v>
+      </c>
+      <c r="J30">
+        <v>152.35677430000001</v>
+      </c>
+      <c r="K30" s="2">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>62.833710979999999</v>
+      </c>
+      <c r="N30">
+        <v>152.35677430000001</v>
+      </c>
+      <c r="O30" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q30">
+        <v>62.833710979999999</v>
+      </c>
+      <c r="R30">
+        <v>152.35677430000001</v>
+      </c>
+      <c r="S30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>74</v>
       </c>
@@ -4278,9 +6359,38 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="G31" s="13"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G31" s="13">
+        <v>7</v>
+      </c>
+      <c r="I31">
+        <v>44.060143920000002</v>
+      </c>
+      <c r="J31">
+        <v>-179.76689150000001</v>
+      </c>
+      <c r="K31" s="2">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>44.060143920000002</v>
+      </c>
+      <c r="N31">
+        <v>-179.76689150000001</v>
+      </c>
+      <c r="O31" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q31">
+        <v>44.060143920000002</v>
+      </c>
+      <c r="R31">
+        <v>-179.76689150000001</v>
+      </c>
+      <c r="S31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>77</v>
       </c>
@@ -4300,9 +6410,38 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="G32" s="13"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G32" s="13">
+        <v>7</v>
+      </c>
+      <c r="I32">
+        <v>55.076595410000003</v>
+      </c>
+      <c r="J32">
+        <v>101.4122131</v>
+      </c>
+      <c r="K32" s="7">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>55.076595410000003</v>
+      </c>
+      <c r="N32">
+        <v>101.4122131</v>
+      </c>
+      <c r="O32" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q32">
+        <v>55.076595410000003</v>
+      </c>
+      <c r="R32">
+        <v>101.4122131</v>
+      </c>
+      <c r="S32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>78</v>
       </c>
@@ -4322,9 +6461,38 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="G33" s="13"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G33" s="13">
+        <v>7</v>
+      </c>
+      <c r="I33">
+        <v>52.46597646</v>
+      </c>
+      <c r="J33">
+        <v>119.9713378</v>
+      </c>
+      <c r="K33" s="7">
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <v>52.46597646</v>
+      </c>
+      <c r="N33">
+        <v>119.9713378</v>
+      </c>
+      <c r="O33" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q33">
+        <v>52.46597646</v>
+      </c>
+      <c r="R33">
+        <v>119.9713378</v>
+      </c>
+      <c r="S33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>79</v>
       </c>
@@ -4344,9 +6512,38 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="G34" s="13"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G34" s="13">
+        <v>7</v>
+      </c>
+      <c r="I34">
+        <v>46.883910020000002</v>
+      </c>
+      <c r="J34">
+        <v>139.31174440000001</v>
+      </c>
+      <c r="K34" s="6">
+        <v>2</v>
+      </c>
+      <c r="M34">
+        <v>46.883910020000002</v>
+      </c>
+      <c r="N34">
+        <v>139.31174440000001</v>
+      </c>
+      <c r="O34" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q34">
+        <v>46.883910020000002</v>
+      </c>
+      <c r="R34">
+        <v>139.31174440000001</v>
+      </c>
+      <c r="S34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>80</v>
       </c>
@@ -4366,9 +6563,38 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="G35" s="13"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G35" s="13">
+        <v>7</v>
+      </c>
+      <c r="I35">
+        <v>46.73331537</v>
+      </c>
+      <c r="J35">
+        <v>119.5303636</v>
+      </c>
+      <c r="K35" s="7">
+        <v>1</v>
+      </c>
+      <c r="M35">
+        <v>46.73331537</v>
+      </c>
+      <c r="N35">
+        <v>119.5303636</v>
+      </c>
+      <c r="O35" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q35">
+        <v>46.73331537</v>
+      </c>
+      <c r="R35">
+        <v>119.5303636</v>
+      </c>
+      <c r="S35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>81</v>
       </c>
@@ -4388,9 +6614,38 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="G36" s="13"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G36" s="13">
+        <v>7</v>
+      </c>
+      <c r="I36">
+        <v>64.607379120000004</v>
+      </c>
+      <c r="J36">
+        <v>138.4237263</v>
+      </c>
+      <c r="K36" s="2">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>64.607379120000004</v>
+      </c>
+      <c r="N36">
+        <v>138.4237263</v>
+      </c>
+      <c r="O36" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q36">
+        <v>64.607379120000004</v>
+      </c>
+      <c r="R36">
+        <v>138.4237263</v>
+      </c>
+      <c r="S36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>83</v>
       </c>
@@ -4410,9 +6665,38 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="G37" s="13"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G37" s="13">
+        <v>7</v>
+      </c>
+      <c r="I37">
+        <v>55.97507701</v>
+      </c>
+      <c r="J37">
+        <v>164.53513720000001</v>
+      </c>
+      <c r="K37" s="2">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>55.97507701</v>
+      </c>
+      <c r="N37">
+        <v>164.53513720000001</v>
+      </c>
+      <c r="O37" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q37">
+        <v>55.97507701</v>
+      </c>
+      <c r="R37">
+        <v>164.53513720000001</v>
+      </c>
+      <c r="S37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>85</v>
       </c>
@@ -4432,9 +6716,38 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="G38" s="13"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G38" s="13">
+        <v>7</v>
+      </c>
+      <c r="I38">
+        <v>54.225132270000003</v>
+      </c>
+      <c r="J38">
+        <v>102.1054611</v>
+      </c>
+      <c r="K38" s="7">
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <v>54.225132270000003</v>
+      </c>
+      <c r="N38">
+        <v>102.1054611</v>
+      </c>
+      <c r="O38" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q38">
+        <v>54.225132270000003</v>
+      </c>
+      <c r="R38">
+        <v>102.1054611</v>
+      </c>
+      <c r="S38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>86</v>
       </c>
@@ -4454,9 +6767,38 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="G39" s="13"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G39" s="13">
+        <v>7</v>
+      </c>
+      <c r="I39">
+        <v>46.274060149999997</v>
+      </c>
+      <c r="J39">
+        <v>102.7464243</v>
+      </c>
+      <c r="K39" s="7">
+        <v>1</v>
+      </c>
+      <c r="M39">
+        <v>46.274060149999997</v>
+      </c>
+      <c r="N39">
+        <v>102.7464243</v>
+      </c>
+      <c r="O39" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q39">
+        <v>46.274060149999997</v>
+      </c>
+      <c r="R39">
+        <v>102.7464243</v>
+      </c>
+      <c r="S39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>88</v>
       </c>
@@ -4476,9 +6818,38 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="G40" s="13"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G40" s="13">
+        <v>7</v>
+      </c>
+      <c r="I40">
+        <v>62.611046379999998</v>
+      </c>
+      <c r="J40">
+        <v>134.7758149</v>
+      </c>
+      <c r="K40" s="2">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>62.611046379999998</v>
+      </c>
+      <c r="N40">
+        <v>134.7758149</v>
+      </c>
+      <c r="O40" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q40">
+        <v>62.611046379999998</v>
+      </c>
+      <c r="R40">
+        <v>134.7758149</v>
+      </c>
+      <c r="S40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>90</v>
       </c>
@@ -4498,7 +6869,36 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="G41" s="13"/>
+      <c r="G41" s="13">
+        <v>7</v>
+      </c>
+      <c r="I41">
+        <v>63.76271208</v>
+      </c>
+      <c r="J41">
+        <v>110.4342592</v>
+      </c>
+      <c r="K41" s="2">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>63.76271208</v>
+      </c>
+      <c r="N41">
+        <v>110.4342592</v>
+      </c>
+      <c r="O41" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q41">
+        <v>63.76271208</v>
+      </c>
+      <c r="R41">
+        <v>110.4342592</v>
+      </c>
+      <c r="S41">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>